<commit_message>
Updating website for pushes
</commit_message>
<xml_diff>
--- a/StructureDefinition-cbs-lab-observation.xlsx
+++ b/StructureDefinition-cbs-lab-observation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="465">
   <si>
     <t>Path</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t>Need to track the status of individual results. Some results are finalized before the whole report is finalized.</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
   <si>
     <t>required</t>
@@ -3202,7 +3205,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" hidden="true">
+    <row r="14">
       <c r="A14" t="s" s="2">
         <v>139</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>55</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>56</v>
@@ -3249,7 +3252,7 @@
         <v>45</v>
       </c>
       <c r="R14" t="s" s="2">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="S14" t="s" s="2">
         <v>45</v>
@@ -3264,13 +3267,13 @@
         <v>45</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>45</v>
@@ -3303,19 +3306,19 @@
         <v>67</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>45</v>
@@ -3323,7 +3326,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3346,19 +3349,19 @@
         <v>45</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>45</v>
@@ -3368,7 +3371,7 @@
         <v>45</v>
       </c>
       <c r="R15" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="S15" t="s" s="2">
         <v>45</v>
@@ -3386,10 +3389,10 @@
         <v>79</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3407,7 +3410,7 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>43</v>
@@ -3431,10 +3434,10 @@
         <v>45</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3442,11 +3445,11 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3465,19 +3468,19 @@
         <v>56</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3502,11 +3505,11 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3524,7 +3527,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>55</v>
@@ -3539,27 +3542,27 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3582,19 +3585,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3643,7 +3646,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3658,19 +3661,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3678,7 +3681,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3701,16 +3704,16 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3760,7 +3763,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3781,13 +3784,13 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3795,11 +3798,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3818,19 +3821,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3879,7 +3882,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3894,19 +3897,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3914,11 +3917,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3937,19 +3940,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3986,17 +3989,17 @@
         <v>45</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AB20" s="2"/>
       <c r="AC20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -4011,19 +4014,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -4031,13 +4034,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -4056,19 +4059,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -4117,7 +4120,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -4132,19 +4135,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4152,7 +4155,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4175,16 +4178,16 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -4234,7 +4237,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4255,13 +4258,13 @@
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4269,7 +4272,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4292,17 +4295,17 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4351,7 +4354,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4366,19 +4369,19 @@
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4386,7 +4389,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4409,19 +4412,19 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4458,17 +4461,17 @@
         <v>45</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AB24" s="2"/>
       <c r="AC24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4477,7 +4480,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4486,27 +4489,27 @@
         <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>45</v>
@@ -4528,19 +4531,19 @@
         <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4589,7 +4592,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4598,7 +4601,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4607,24 +4610,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4650,10 +4653,10 @@
         <v>57</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4704,7 +4707,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4728,7 +4731,7 @@
         <v>45</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4739,7 +4742,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4768,7 +4771,7 @@
         <v>102</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M27" t="s" s="2">
         <v>104</v>
@@ -4809,19 +4812,19 @@
         <v>45</v>
       </c>
       <c r="AA27" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AB27" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AC27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD27" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4845,7 +4848,7 @@
         <v>45</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
@@ -4856,7 +4859,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4879,19 +4882,19 @@
         <v>56</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4940,7 +4943,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4961,10 +4964,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4975,7 +4978,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5001,20 +5004,20 @@
         <v>75</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P29" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="Q29" t="s" s="2">
         <v>45</v>
@@ -5035,13 +5038,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -5059,7 +5062,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -5080,10 +5083,10 @@
         <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
@@ -5094,7 +5097,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5120,14 +5123,14 @@
         <v>57</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -5176,7 +5179,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5197,10 +5200,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5211,7 +5214,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5237,14 +5240,14 @@
         <v>69</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5293,7 +5296,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5302,7 +5305,7 @@
         <v>55</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>67</v>
@@ -5314,10 +5317,10 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5328,7 +5331,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5354,16 +5357,16 @@
         <v>75</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
@@ -5412,7 +5415,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5433,10 +5436,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5447,10 +5450,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>45</v>
@@ -5472,19 +5475,19 @@
         <v>56</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5509,11 +5512,11 @@
         <v>45</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X33" s="2"/>
       <c r="Y33" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>45</v>
@@ -5531,7 +5534,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5540,7 +5543,7 @@
         <v>55</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>67</v>
@@ -5549,27 +5552,27 @@
         <v>45</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>45</v>
@@ -5594,16 +5597,16 @@
         <v>57</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5652,7 +5655,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5661,7 +5664,7 @@
         <v>55</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>67</v>
@@ -5670,24 +5673,24 @@
         <v>45</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5710,19 +5713,19 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
@@ -5747,13 +5750,13 @@
         <v>45</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>45</v>
@@ -5771,7 +5774,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5780,7 +5783,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5795,7 +5798,7 @@
         <v>98</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5806,11 +5809,11 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -5829,19 +5832,19 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5866,13 +5869,13 @@
         <v>45</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
@@ -5890,7 +5893,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5908,24 +5911,24 @@
         <v>45</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5948,19 +5951,19 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -6009,7 +6012,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -6030,10 +6033,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -6044,7 +6047,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6067,16 +6070,16 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -6102,13 +6105,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -6126,7 +6129,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6144,24 +6147,24 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6184,19 +6187,19 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6221,13 +6224,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6245,7 +6248,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6266,10 +6269,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6280,7 +6283,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6303,16 +6306,16 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
@@ -6362,7 +6365,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6380,24 +6383,24 @@
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6420,16 +6423,16 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6479,7 +6482,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6497,24 +6500,24 @@
         <v>45</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6537,19 +6540,19 @@
         <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>45</v>
@@ -6598,7 +6601,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6610,7 +6613,7 @@
         <v>45</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>45</v>
@@ -6619,10 +6622,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6633,7 +6636,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6659,10 +6662,10 @@
         <v>57</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6713,7 +6716,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6737,7 +6740,7 @@
         <v>45</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6748,7 +6751,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6777,7 +6780,7 @@
         <v>102</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M44" t="s" s="2">
         <v>104</v>
@@ -6830,7 +6833,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6854,7 +6857,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6865,11 +6868,11 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -6891,10 +6894,10 @@
         <v>101</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6949,7 +6952,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6984,7 +6987,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7007,13 +7010,13 @@
         <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -7064,7 +7067,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7073,7 +7076,7 @@
         <v>55</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>67</v>
@@ -7085,10 +7088,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -7099,7 +7102,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7122,13 +7125,13 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -7179,7 +7182,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7188,7 +7191,7 @@
         <v>55</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>67</v>
@@ -7200,10 +7203,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7214,7 +7217,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7237,19 +7240,19 @@
         <v>45</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7277,10 +7280,10 @@
         <v>79</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7298,7 +7301,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7316,13 +7319,13 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7333,7 +7336,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7356,19 +7359,19 @@
         <v>45</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7393,13 +7396,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7417,7 +7420,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7435,13 +7438,13 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7452,7 +7455,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7475,17 +7478,17 @@
         <v>45</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7534,7 +7537,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7558,7 +7561,7 @@
         <v>45</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
@@ -7569,7 +7572,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7595,10 +7598,10 @@
         <v>57</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7649,7 +7652,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7670,10 +7673,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7684,7 +7687,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7707,16 +7710,16 @@
         <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7766,7 +7769,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7787,10 +7790,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7801,7 +7804,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7824,16 +7827,16 @@
         <v>56</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
@@ -7883,7 +7886,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7904,10 +7907,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -7918,7 +7921,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7941,19 +7944,19 @@
         <v>56</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -8002,7 +8005,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8023,10 +8026,10 @@
         <v>45</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8037,7 +8040,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8063,10 +8066,10 @@
         <v>57</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -8117,7 +8120,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8141,7 +8144,7 @@
         <v>45</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8152,7 +8155,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8181,7 +8184,7 @@
         <v>102</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M56" t="s" s="2">
         <v>104</v>
@@ -8234,7 +8237,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8258,7 +8261,7 @@
         <v>45</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
@@ -8269,11 +8272,11 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -8295,10 +8298,10 @@
         <v>101</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M57" t="s" s="2">
         <v>104</v>
@@ -8353,7 +8356,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8388,7 +8391,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8411,19 +8414,19 @@
         <v>56</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8448,13 +8451,13 @@
         <v>45</v>
       </c>
       <c r="W58" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>45</v>
@@ -8472,7 +8475,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>55</v>
@@ -8490,16 +8493,16 @@
         <v>45</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AO58" t="s" s="2">
         <v>45</v>
@@ -8507,7 +8510,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8530,19 +8533,19 @@
         <v>56</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8591,7 +8594,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8609,24 +8612,24 @@
         <v>45</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8649,19 +8652,19 @@
         <v>45</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>45</v>
@@ -8686,13 +8689,13 @@
         <v>45</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>45</v>
@@ -8710,7 +8713,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -8719,7 +8722,7 @@
         <v>55</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>67</v>
@@ -8734,7 +8737,7 @@
         <v>98</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
@@ -8745,11 +8748,11 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
@@ -8768,19 +8771,19 @@
         <v>45</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -8805,13 +8808,13 @@
         <v>45</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>45</v>
@@ -8829,7 +8832,7 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -8847,24 +8850,24 @@
         <v>45</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO61" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8890,16 +8893,16 @@
         <v>45</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
@@ -8948,7 +8951,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -8969,10 +8972,10 @@
         <v>45</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>45</v>

</xml_diff>